<commit_message>
new version iq and urgency
</commit_message>
<xml_diff>
--- a/fhir/ig/iq/CodeSystem-CSPractitionerTipoRolLE.xlsx
+++ b/fhir/ig/iq/CodeSystem-CSPractitionerTipoRolLE.xlsx
@@ -147,10 +147,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>iniciador</t>
-  </si>
-  <si>
-    <t>Iniciador</t>
+    <t>indicador</t>
+  </si>
+  <si>
+    <t>Indicador</t>
   </si>
   <si>
     <t>Médico cirujano u odontólogo con especialidad quirúrgica a cargo de realizar la indicación de cirugía, y la priorización. Actúa dentro del evento atender.</t>

</xml_diff>